<commit_message>
Added a cleaned data file
</commit_message>
<xml_diff>
--- a/Data/WineQT.xlsx
+++ b/Data/WineQT.xlsx
@@ -884,7 +884,7 @@
         <v>1.8</v>
       </c>
       <c r="E11" t="n">
-        <v>0.097</v>
+        <v>0.09699999999999991</v>
       </c>
       <c r="F11" t="n">
         <v>15</v>
@@ -925,7 +925,7 @@
         <v>1.6</v>
       </c>
       <c r="E12" t="n">
-        <v>0.08900000000000001</v>
+        <v>0.089</v>
       </c>
       <c r="F12" t="n">
         <v>16</v>
@@ -1089,7 +1089,7 @@
         <v>2.3</v>
       </c>
       <c r="E16" t="n">
-        <v>0.08199999999999999</v>
+        <v>0.08199999999999991</v>
       </c>
       <c r="F16" t="n">
         <v>23</v>
@@ -1376,7 +1376,7 @@
         <v>2</v>
       </c>
       <c r="E23" t="n">
-        <v>0.08199999999999999</v>
+        <v>0.08199999999999991</v>
       </c>
       <c r="F23" t="n">
         <v>8</v>
@@ -1417,7 +1417,7 @@
         <v>2.4</v>
       </c>
       <c r="E24" t="n">
-        <v>0.08900000000000001</v>
+        <v>0.089</v>
       </c>
       <c r="F24" t="n">
         <v>17</v>
@@ -1663,7 +1663,7 @@
         <v>5.9</v>
       </c>
       <c r="E30" t="n">
-        <v>0.07400000000000001</v>
+        <v>0.074</v>
       </c>
       <c r="F30" t="n">
         <v>12</v>
@@ -1704,7 +1704,7 @@
         <v>2.8</v>
       </c>
       <c r="E31" t="n">
-        <v>0.08800000000000001</v>
+        <v>0.08799999999999999</v>
       </c>
       <c r="F31" t="n">
         <v>17</v>
@@ -1827,7 +1827,7 @@
         <v>2.1</v>
       </c>
       <c r="E34" t="n">
-        <v>0.05400000000000001</v>
+        <v>0.054</v>
       </c>
       <c r="F34" t="n">
         <v>8</v>
@@ -1909,7 +1909,7 @@
         <v>1.7</v>
       </c>
       <c r="E36" t="n">
-        <v>0.07400000000000001</v>
+        <v>0.074</v>
       </c>
       <c r="F36" t="n">
         <v>4</v>
@@ -2196,7 +2196,7 @@
         <v>2.4</v>
       </c>
       <c r="E43" t="n">
-        <v>0.07400000000000001</v>
+        <v>0.074</v>
       </c>
       <c r="F43" t="n">
         <v>9</v>
@@ -2483,7 +2483,7 @@
         <v>1.9</v>
       </c>
       <c r="E50" t="n">
-        <v>0.07400000000000001</v>
+        <v>0.074</v>
       </c>
       <c r="F50" t="n">
         <v>8</v>
@@ -3631,7 +3631,7 @@
         <v>1.7</v>
       </c>
       <c r="E78" t="n">
-        <v>0.08800000000000001</v>
+        <v>0.08799999999999999</v>
       </c>
       <c r="F78" t="n">
         <v>15</v>
@@ -4041,7 +4041,7 @@
         <v>1.6</v>
       </c>
       <c r="E88" t="n">
-        <v>0.08199999999999999</v>
+        <v>0.08199999999999991</v>
       </c>
       <c r="F88" t="n">
         <v>21</v>
@@ -4123,7 +4123,7 @@
         <v>1.8</v>
       </c>
       <c r="E90" t="n">
-        <v>0.08199999999999999</v>
+        <v>0.08199999999999991</v>
       </c>
       <c r="F90" t="n">
         <v>3</v>
@@ -4574,7 +4574,7 @@
         <v>1.8</v>
       </c>
       <c r="E101" t="n">
-        <v>0.117</v>
+        <v>0.1169999999999999</v>
       </c>
       <c r="F101" t="n">
         <v>32</v>
@@ -4656,7 +4656,7 @@
         <v>2.3</v>
       </c>
       <c r="E103" t="n">
-        <v>0.07400000000000001</v>
+        <v>0.074</v>
       </c>
       <c r="F103" t="n">
         <v>12</v>
@@ -5107,7 +5107,7 @@
         <v>1.3</v>
       </c>
       <c r="E114" t="n">
-        <v>0.07200000000000001</v>
+        <v>0.07199999999999999</v>
       </c>
       <c r="F114" t="n">
         <v>9</v>
@@ -5353,7 +5353,7 @@
         <v>1.6</v>
       </c>
       <c r="E120" t="n">
-        <v>0.07200000000000001</v>
+        <v>0.07199999999999999</v>
       </c>
       <c r="F120" t="n">
         <v>17</v>
@@ -5394,7 +5394,7 @@
         <v>2.1</v>
       </c>
       <c r="E121" t="n">
-        <v>0.08900000000000001</v>
+        <v>0.089</v>
       </c>
       <c r="F121" t="n">
         <v>11</v>
@@ -5435,7 +5435,7 @@
         <v>1.8</v>
       </c>
       <c r="E122" t="n">
-        <v>0.058</v>
+        <v>0.0579999999999999</v>
       </c>
       <c r="F122" t="n">
         <v>4</v>
@@ -6009,7 +6009,7 @@
         <v>2</v>
       </c>
       <c r="E136" t="n">
-        <v>0.08199999999999999</v>
+        <v>0.08199999999999991</v>
       </c>
       <c r="F136" t="n">
         <v>14</v>
@@ -6132,7 +6132,7 @@
         <v>1.9</v>
       </c>
       <c r="E139" t="n">
-        <v>0.07400000000000001</v>
+        <v>0.074</v>
       </c>
       <c r="F139" t="n">
         <v>21</v>
@@ -6255,7 +6255,7 @@
         <v>2.4</v>
       </c>
       <c r="E142" t="n">
-        <v>0.07400000000000001</v>
+        <v>0.074</v>
       </c>
       <c r="F142" t="n">
         <v>15</v>
@@ -6378,7 +6378,7 @@
         <v>1.4</v>
       </c>
       <c r="E145" t="n">
-        <v>0.056</v>
+        <v>0.0559999999999999</v>
       </c>
       <c r="F145" t="n">
         <v>9</v>
@@ -6419,7 +6419,7 @@
         <v>1.6</v>
       </c>
       <c r="E146" t="n">
-        <v>0.08900000000000001</v>
+        <v>0.089</v>
       </c>
       <c r="F146" t="n">
         <v>14</v>
@@ -6788,7 +6788,7 @@
         <v>2</v>
       </c>
       <c r="E155" t="n">
-        <v>0.101</v>
+        <v>0.1009999999999999</v>
       </c>
       <c r="F155" t="n">
         <v>13</v>
@@ -6829,7 +6829,7 @@
         <v>2.2</v>
       </c>
       <c r="E156" t="n">
-        <v>0.07200000000000001</v>
+        <v>0.07199999999999999</v>
       </c>
       <c r="F156" t="n">
         <v>11</v>
@@ -6911,7 +6911,7 @@
         <v>2</v>
       </c>
       <c r="E158" t="n">
-        <v>0.08199999999999999</v>
+        <v>0.08199999999999991</v>
       </c>
       <c r="F158" t="n">
         <v>24</v>
@@ -6952,7 +6952,7 @@
         <v>2</v>
       </c>
       <c r="E159" t="n">
-        <v>0.101</v>
+        <v>0.1009999999999999</v>
       </c>
       <c r="F159" t="n">
         <v>16</v>
@@ -7157,7 +7157,7 @@
         <v>1.6</v>
       </c>
       <c r="E164" t="n">
-        <v>0.05400000000000001</v>
+        <v>0.054</v>
       </c>
       <c r="F164" t="n">
         <v>19</v>
@@ -7321,7 +7321,7 @@
         <v>1.9</v>
       </c>
       <c r="E168" t="n">
-        <v>0.097</v>
+        <v>0.09699999999999991</v>
       </c>
       <c r="F168" t="n">
         <v>14</v>
@@ -7731,7 +7731,7 @@
         <v>1.8</v>
       </c>
       <c r="E178" t="n">
-        <v>0.07400000000000001</v>
+        <v>0.074</v>
       </c>
       <c r="F178" t="n">
         <v>16</v>
@@ -9494,7 +9494,7 @@
         <v>2.1</v>
       </c>
       <c r="E221" t="n">
-        <v>0.112</v>
+        <v>0.1119999999999999</v>
       </c>
       <c r="F221" t="n">
         <v>12</v>
@@ -9535,7 +9535,7 @@
         <v>2.2</v>
       </c>
       <c r="E222" t="n">
-        <v>0.08199999999999999</v>
+        <v>0.08199999999999991</v>
       </c>
       <c r="F222" t="n">
         <v>7</v>
@@ -9658,7 +9658,7 @@
         <v>2</v>
       </c>
       <c r="E225" t="n">
-        <v>0.07200000000000001</v>
+        <v>0.07199999999999999</v>
       </c>
       <c r="F225" t="n">
         <v>15</v>
@@ -9863,7 +9863,7 @@
         <v>2.9</v>
       </c>
       <c r="E230" t="n">
-        <v>0.08199999999999999</v>
+        <v>0.08199999999999991</v>
       </c>
       <c r="F230" t="n">
         <v>30</v>
@@ -10109,7 +10109,7 @@
         <v>2.6</v>
       </c>
       <c r="E236" t="n">
-        <v>0.08199999999999999</v>
+        <v>0.08199999999999991</v>
       </c>
       <c r="F236" t="n">
         <v>6</v>
@@ -10355,7 +10355,7 @@
         <v>2.3</v>
       </c>
       <c r="E242" t="n">
-        <v>0.08199999999999999</v>
+        <v>0.08199999999999991</v>
       </c>
       <c r="F242" t="n">
         <v>12</v>
@@ -10478,7 +10478,7 @@
         <v>2.6</v>
       </c>
       <c r="E245" t="n">
-        <v>0.08199999999999999</v>
+        <v>0.08199999999999991</v>
       </c>
       <c r="F245" t="n">
         <v>6</v>
@@ -10560,7 +10560,7 @@
         <v>2.8</v>
       </c>
       <c r="E247" t="n">
-        <v>0.08900000000000001</v>
+        <v>0.089</v>
       </c>
       <c r="F247" t="n">
         <v>15</v>
@@ -10847,7 +10847,7 @@
         <v>2.95</v>
       </c>
       <c r="E254" t="n">
-        <v>0.116</v>
+        <v>0.1159999999999999</v>
       </c>
       <c r="F254" t="n">
         <v>12</v>
@@ -10929,7 +10929,7 @@
         <v>2.6</v>
       </c>
       <c r="E256" t="n">
-        <v>0.08800000000000001</v>
+        <v>0.08799999999999999</v>
       </c>
       <c r="F256" t="n">
         <v>10</v>
@@ -11052,7 +11052,7 @@
         <v>2.5</v>
       </c>
       <c r="E259" t="n">
-        <v>0.07200000000000001</v>
+        <v>0.07199999999999999</v>
       </c>
       <c r="F259" t="n">
         <v>6</v>
@@ -11257,7 +11257,7 @@
         <v>2.4</v>
       </c>
       <c r="E264" t="n">
-        <v>0.07400000000000001</v>
+        <v>0.074</v>
       </c>
       <c r="F264" t="n">
         <v>6</v>
@@ -11298,7 +11298,7 @@
         <v>1.6</v>
       </c>
       <c r="E265" t="n">
-        <v>0.056</v>
+        <v>0.0559999999999999</v>
       </c>
       <c r="F265" t="n">
         <v>11</v>
@@ -11421,7 +11421,7 @@
         <v>2.4</v>
       </c>
       <c r="E268" t="n">
-        <v>0.07400000000000001</v>
+        <v>0.074</v>
       </c>
       <c r="F268" t="n">
         <v>6</v>
@@ -11462,7 +11462,7 @@
         <v>6.2</v>
       </c>
       <c r="E269" t="n">
-        <v>0.08800000000000001</v>
+        <v>0.08799999999999999</v>
       </c>
       <c r="F269" t="n">
         <v>6</v>
@@ -11585,7 +11585,7 @@
         <v>1.9</v>
       </c>
       <c r="E272" t="n">
-        <v>0.08800000000000001</v>
+        <v>0.08799999999999999</v>
       </c>
       <c r="F272" t="n">
         <v>23</v>
@@ -11708,7 +11708,7 @@
         <v>2</v>
       </c>
       <c r="E275" t="n">
-        <v>0.08199999999999999</v>
+        <v>0.08199999999999991</v>
       </c>
       <c r="F275" t="n">
         <v>6</v>
@@ -12282,7 +12282,7 @@
         <v>6.7</v>
       </c>
       <c r="E289" t="n">
-        <v>0.097</v>
+        <v>0.09699999999999991</v>
       </c>
       <c r="F289" t="n">
         <v>6</v>
@@ -12364,7 +12364,7 @@
         <v>6.6</v>
       </c>
       <c r="E291" t="n">
-        <v>0.117</v>
+        <v>0.1169999999999999</v>
       </c>
       <c r="F291" t="n">
         <v>31</v>
@@ -12856,7 +12856,7 @@
         <v>2.4</v>
       </c>
       <c r="E303" t="n">
-        <v>0.08800000000000001</v>
+        <v>0.08799999999999999</v>
       </c>
       <c r="F303" t="n">
         <v>13</v>
@@ -12938,7 +12938,7 @@
         <v>2.2</v>
       </c>
       <c r="E305" t="n">
-        <v>0.07400000000000001</v>
+        <v>0.074</v>
       </c>
       <c r="F305" t="n">
         <v>21</v>
@@ -13225,7 +13225,7 @@
         <v>2.2</v>
       </c>
       <c r="E312" t="n">
-        <v>0.07200000000000001</v>
+        <v>0.07199999999999999</v>
       </c>
       <c r="F312" t="n">
         <v>6</v>
@@ -13307,7 +13307,7 @@
         <v>1.7</v>
       </c>
       <c r="E314" t="n">
-        <v>0.05400000000000001</v>
+        <v>0.054</v>
       </c>
       <c r="F314" t="n">
         <v>5</v>
@@ -13758,7 +13758,7 @@
         <v>2.7</v>
       </c>
       <c r="E325" t="n">
-        <v>0.097</v>
+        <v>0.09699999999999991</v>
       </c>
       <c r="F325" t="n">
         <v>29</v>
@@ -13799,7 +13799,7 @@
         <v>2.2</v>
       </c>
       <c r="E326" t="n">
-        <v>0.07400000000000001</v>
+        <v>0.074</v>
       </c>
       <c r="F326" t="n">
         <v>10</v>
@@ -14537,7 +14537,7 @@
         <v>1.9</v>
       </c>
       <c r="E344" t="n">
-        <v>0.05400000000000001</v>
+        <v>0.054</v>
       </c>
       <c r="F344" t="n">
         <v>6</v>
@@ -15070,7 +15070,7 @@
         <v>6.55</v>
       </c>
       <c r="E357" t="n">
-        <v>0.07400000000000001</v>
+        <v>0.074</v>
       </c>
       <c r="F357" t="n">
         <v>38</v>
@@ -15111,7 +15111,7 @@
         <v>6.55</v>
       </c>
       <c r="E358" t="n">
-        <v>0.07400000000000001</v>
+        <v>0.074</v>
       </c>
       <c r="F358" t="n">
         <v>38</v>
@@ -15193,7 +15193,7 @@
         <v>2.9</v>
       </c>
       <c r="E360" t="n">
-        <v>0.07200000000000001</v>
+        <v>0.07199999999999999</v>
       </c>
       <c r="F360" t="n">
         <v>10</v>
@@ -15644,7 +15644,7 @@
         <v>2.7</v>
       </c>
       <c r="E371" t="n">
-        <v>0.08800000000000001</v>
+        <v>0.08799999999999999</v>
       </c>
       <c r="F371" t="n">
         <v>15</v>
@@ -15767,7 +15767,7 @@
         <v>2.5</v>
       </c>
       <c r="E374" t="n">
-        <v>0.097</v>
+        <v>0.09699999999999991</v>
       </c>
       <c r="F374" t="n">
         <v>33</v>
@@ -15972,7 +15972,7 @@
         <v>2.1</v>
       </c>
       <c r="E379" t="n">
-        <v>0.07200000000000001</v>
+        <v>0.07199999999999999</v>
       </c>
       <c r="F379" t="n">
         <v>15</v>
@@ -16259,7 +16259,7 @@
         <v>3.3</v>
       </c>
       <c r="E386" t="n">
-        <v>0.101</v>
+        <v>0.1009999999999999</v>
       </c>
       <c r="F386" t="n">
         <v>20</v>
@@ -16628,7 +16628,7 @@
         <v>2.1</v>
       </c>
       <c r="E395" t="n">
-        <v>0.07400000000000001</v>
+        <v>0.074</v>
       </c>
       <c r="F395" t="n">
         <v>9</v>
@@ -17530,7 +17530,7 @@
         <v>2.2</v>
       </c>
       <c r="E417" t="n">
-        <v>0.08900000000000001</v>
+        <v>0.089</v>
       </c>
       <c r="F417" t="n">
         <v>5</v>
@@ -17571,7 +17571,7 @@
         <v>2.2</v>
       </c>
       <c r="E418" t="n">
-        <v>0.08900000000000001</v>
+        <v>0.089</v>
       </c>
       <c r="F418" t="n">
         <v>5</v>
@@ -17612,7 +17612,7 @@
         <v>1.9</v>
       </c>
       <c r="E419" t="n">
-        <v>0.07400000000000001</v>
+        <v>0.074</v>
       </c>
       <c r="F419" t="n">
         <v>10</v>
@@ -18432,7 +18432,7 @@
         <v>2.3</v>
       </c>
       <c r="E439" t="n">
-        <v>0.08800000000000001</v>
+        <v>0.08799999999999999</v>
       </c>
       <c r="F439" t="n">
         <v>6</v>
@@ -18719,7 +18719,7 @@
         <v>2.5</v>
       </c>
       <c r="E446" t="n">
-        <v>0.097</v>
+        <v>0.09699999999999991</v>
       </c>
       <c r="F446" t="n">
         <v>7</v>
@@ -18801,7 +18801,7 @@
         <v>2.5</v>
       </c>
       <c r="E448" t="n">
-        <v>0.097</v>
+        <v>0.09699999999999991</v>
       </c>
       <c r="F448" t="n">
         <v>7</v>
@@ -19539,7 +19539,7 @@
         <v>2.4</v>
       </c>
       <c r="E466" t="n">
-        <v>0.07400000000000001</v>
+        <v>0.074</v>
       </c>
       <c r="F466" t="n">
         <v>7</v>
@@ -19703,7 +19703,7 @@
         <v>1.4</v>
       </c>
       <c r="E470" t="n">
-        <v>0.07400000000000001</v>
+        <v>0.074</v>
       </c>
       <c r="F470" t="n">
         <v>5</v>
@@ -19744,7 +19744,7 @@
         <v>1.4</v>
       </c>
       <c r="E471" t="n">
-        <v>0.07400000000000001</v>
+        <v>0.074</v>
       </c>
       <c r="F471" t="n">
         <v>5</v>
@@ -19949,7 +19949,7 @@
         <v>2</v>
       </c>
       <c r="E476" t="n">
-        <v>0.08199999999999999</v>
+        <v>0.08199999999999991</v>
       </c>
       <c r="F476" t="n">
         <v>6</v>
@@ -19990,7 +19990,7 @@
         <v>2</v>
       </c>
       <c r="E477" t="n">
-        <v>0.08199999999999999</v>
+        <v>0.08199999999999991</v>
       </c>
       <c r="F477" t="n">
         <v>6</v>
@@ -20031,7 +20031,7 @@
         <v>1.7</v>
       </c>
       <c r="E478" t="n">
-        <v>0.07400000000000001</v>
+        <v>0.074</v>
       </c>
       <c r="F478" t="n">
         <v>5</v>
@@ -20072,7 +20072,7 @@
         <v>1.7</v>
       </c>
       <c r="E479" t="n">
-        <v>0.07400000000000001</v>
+        <v>0.074</v>
       </c>
       <c r="F479" t="n">
         <v>5</v>
@@ -21425,7 +21425,7 @@
         <v>2</v>
       </c>
       <c r="E512" t="n">
-        <v>0.08199999999999999</v>
+        <v>0.08199999999999991</v>
       </c>
       <c r="F512" t="n">
         <v>10</v>
@@ -21507,7 +21507,7 @@
         <v>2</v>
       </c>
       <c r="E514" t="n">
-        <v>0.08199999999999999</v>
+        <v>0.08199999999999991</v>
       </c>
       <c r="F514" t="n">
         <v>10</v>
@@ -21876,7 +21876,7 @@
         <v>3.45</v>
       </c>
       <c r="E523" t="n">
-        <v>0.08800000000000001</v>
+        <v>0.08799999999999999</v>
       </c>
       <c r="F523" t="n">
         <v>4</v>
@@ -21958,7 +21958,7 @@
         <v>2.7</v>
       </c>
       <c r="E525" t="n">
-        <v>0.08199999999999999</v>
+        <v>0.08199999999999991</v>
       </c>
       <c r="F525" t="n">
         <v>16</v>
@@ -22040,7 +22040,7 @@
         <v>2.1</v>
       </c>
       <c r="E527" t="n">
-        <v>0.112</v>
+        <v>0.1119999999999999</v>
       </c>
       <c r="F527" t="n">
         <v>11</v>
@@ -22122,7 +22122,7 @@
         <v>2.4</v>
       </c>
       <c r="E529" t="n">
-        <v>0.08800000000000001</v>
+        <v>0.08799999999999999</v>
       </c>
       <c r="F529" t="n">
         <v>19</v>
@@ -22450,7 +22450,7 @@
         <v>2.9</v>
       </c>
       <c r="E537" t="n">
-        <v>0.08900000000000001</v>
+        <v>0.089</v>
       </c>
       <c r="F537" t="n">
         <v>17</v>
@@ -22491,7 +22491,7 @@
         <v>2.5</v>
       </c>
       <c r="E538" t="n">
-        <v>0.097</v>
+        <v>0.09699999999999991</v>
       </c>
       <c r="F538" t="n">
         <v>24</v>
@@ -22532,7 +22532,7 @@
         <v>2.9</v>
       </c>
       <c r="E539" t="n">
-        <v>0.08900000000000001</v>
+        <v>0.089</v>
       </c>
       <c r="F539" t="n">
         <v>17</v>
@@ -22614,7 +22614,7 @@
         <v>1.9</v>
       </c>
       <c r="E541" t="n">
-        <v>0.058</v>
+        <v>0.0579999999999999</v>
       </c>
       <c r="F541" t="n">
         <v>22</v>
@@ -23024,7 +23024,7 @@
         <v>2.9</v>
       </c>
       <c r="E551" t="n">
-        <v>0.08900000000000001</v>
+        <v>0.089</v>
       </c>
       <c r="F551" t="n">
         <v>12</v>
@@ -23065,7 +23065,7 @@
         <v>2.3</v>
       </c>
       <c r="E552" t="n">
-        <v>0.08199999999999999</v>
+        <v>0.08199999999999991</v>
       </c>
       <c r="F552" t="n">
         <v>24</v>
@@ -23147,7 +23147,7 @@
         <v>2.3</v>
       </c>
       <c r="E554" t="n">
-        <v>0.08199999999999999</v>
+        <v>0.08199999999999991</v>
       </c>
       <c r="F554" t="n">
         <v>24</v>
@@ -23188,7 +23188,7 @@
         <v>2.4</v>
       </c>
       <c r="E555" t="n">
-        <v>0.08199999999999999</v>
+        <v>0.08199999999999991</v>
       </c>
       <c r="F555" t="n">
         <v>23</v>
@@ -23229,7 +23229,7 @@
         <v>2.3</v>
       </c>
       <c r="E556" t="n">
-        <v>0.08199999999999999</v>
+        <v>0.08199999999999991</v>
       </c>
       <c r="F556" t="n">
         <v>23</v>
@@ -23762,7 +23762,7 @@
         <v>2.6</v>
       </c>
       <c r="E569" t="n">
-        <v>0.08199999999999999</v>
+        <v>0.08199999999999991</v>
       </c>
       <c r="F569" t="n">
         <v>18</v>
@@ -24090,7 +24090,7 @@
         <v>3.6</v>
       </c>
       <c r="E577" t="n">
-        <v>0.08199999999999999</v>
+        <v>0.08199999999999991</v>
       </c>
       <c r="F577" t="n">
         <v>5</v>
@@ -24295,7 +24295,7 @@
         <v>2</v>
       </c>
       <c r="E582" t="n">
-        <v>0.041</v>
+        <v>0.0409999999999999</v>
       </c>
       <c r="F582" t="n">
         <v>4</v>
@@ -24459,7 +24459,7 @@
         <v>2.8</v>
       </c>
       <c r="E586" t="n">
-        <v>0.07200000000000001</v>
+        <v>0.07199999999999999</v>
       </c>
       <c r="F586" t="n">
         <v>7</v>
@@ -24582,7 +24582,7 @@
         <v>3.2</v>
       </c>
       <c r="E589" t="n">
-        <v>0.097</v>
+        <v>0.09699999999999991</v>
       </c>
       <c r="F589" t="n">
         <v>9</v>
@@ -24869,7 +24869,7 @@
         <v>2.5</v>
       </c>
       <c r="E596" t="n">
-        <v>0.058</v>
+        <v>0.0579999999999999</v>
       </c>
       <c r="F596" t="n">
         <v>5</v>
@@ -25197,7 +25197,7 @@
         <v>2</v>
       </c>
       <c r="E604" t="n">
-        <v>0.08800000000000001</v>
+        <v>0.08799999999999999</v>
       </c>
       <c r="F604" t="n">
         <v>9</v>
@@ -25607,7 +25607,7 @@
         <v>1.7</v>
       </c>
       <c r="E614" t="n">
-        <v>0.05400000000000001</v>
+        <v>0.054</v>
       </c>
       <c r="F614" t="n">
         <v>17</v>
@@ -26017,7 +26017,7 @@
         <v>3.1</v>
       </c>
       <c r="E624" t="n">
-        <v>0.194</v>
+        <v>0.1939999999999999</v>
       </c>
       <c r="F624" t="n">
         <v>14</v>
@@ -26181,7 +26181,7 @@
         <v>2.5</v>
       </c>
       <c r="E628" t="n">
-        <v>0.07200000000000001</v>
+        <v>0.07199999999999999</v>
       </c>
       <c r="F628" t="n">
         <v>32</v>
@@ -26222,7 +26222,7 @@
         <v>6.6</v>
       </c>
       <c r="E629" t="n">
-        <v>0.112</v>
+        <v>0.1119999999999999</v>
       </c>
       <c r="F629" t="n">
         <v>23</v>
@@ -26304,7 +26304,7 @@
         <v>1.9</v>
       </c>
       <c r="E631" t="n">
-        <v>0.08199999999999999</v>
+        <v>0.08199999999999991</v>
       </c>
       <c r="F631" t="n">
         <v>10</v>
@@ -26591,7 +26591,7 @@
         <v>2.6</v>
       </c>
       <c r="E638" t="n">
-        <v>0.056</v>
+        <v>0.0559999999999999</v>
       </c>
       <c r="F638" t="n">
         <v>10</v>
@@ -27165,7 +27165,7 @@
         <v>1.8</v>
       </c>
       <c r="E652" t="n">
-        <v>0.07200000000000001</v>
+        <v>0.07199999999999999</v>
       </c>
       <c r="F652" t="n">
         <v>38</v>
@@ -27247,7 +27247,7 @@
         <v>1.8</v>
       </c>
       <c r="E654" t="n">
-        <v>0.07200000000000001</v>
+        <v>0.07199999999999999</v>
       </c>
       <c r="F654" t="n">
         <v>38</v>
@@ -27534,7 +27534,7 @@
         <v>2</v>
       </c>
       <c r="E661" t="n">
-        <v>0.07400000000000001</v>
+        <v>0.074</v>
       </c>
       <c r="F661" t="n">
         <v>13</v>
@@ -27739,7 +27739,7 @@
         <v>5</v>
       </c>
       <c r="E666" t="n">
-        <v>0.08199999999999999</v>
+        <v>0.08199999999999991</v>
       </c>
       <c r="F666" t="n">
         <v>9</v>
@@ -28067,7 +28067,7 @@
         <v>2.2</v>
       </c>
       <c r="E674" t="n">
-        <v>0.058</v>
+        <v>0.0579999999999999</v>
       </c>
       <c r="F674" t="n">
         <v>6</v>
@@ -28272,7 +28272,7 @@
         <v>1.9</v>
       </c>
       <c r="E679" t="n">
-        <v>0.058</v>
+        <v>0.0579999999999999</v>
       </c>
       <c r="F679" t="n">
         <v>18</v>
@@ -28395,7 +28395,7 @@
         <v>1.9</v>
       </c>
       <c r="E682" t="n">
-        <v>0.058</v>
+        <v>0.0579999999999999</v>
       </c>
       <c r="F682" t="n">
         <v>18</v>
@@ -28436,7 +28436,7 @@
         <v>2.1</v>
       </c>
       <c r="E683" t="n">
-        <v>0.097</v>
+        <v>0.09699999999999991</v>
       </c>
       <c r="F683" t="n">
         <v>23</v>
@@ -28969,7 +28969,7 @@
         <v>1.7</v>
       </c>
       <c r="E696" t="n">
-        <v>0.097</v>
+        <v>0.09699999999999991</v>
       </c>
       <c r="F696" t="n">
         <v>19</v>
@@ -29051,7 +29051,7 @@
         <v>1.7</v>
       </c>
       <c r="E698" t="n">
-        <v>0.097</v>
+        <v>0.09699999999999991</v>
       </c>
       <c r="F698" t="n">
         <v>19</v>
@@ -29092,7 +29092,7 @@
         <v>2</v>
       </c>
       <c r="E699" t="n">
-        <v>0.08199999999999999</v>
+        <v>0.08199999999999991</v>
       </c>
       <c r="F699" t="n">
         <v>31</v>
@@ -29133,7 +29133,7 @@
         <v>2</v>
       </c>
       <c r="E700" t="n">
-        <v>0.08199999999999999</v>
+        <v>0.08199999999999991</v>
       </c>
       <c r="F700" t="n">
         <v>31</v>
@@ -29584,7 +29584,7 @@
         <v>2</v>
       </c>
       <c r="E711" t="n">
-        <v>0.08800000000000001</v>
+        <v>0.08799999999999999</v>
       </c>
       <c r="F711" t="n">
         <v>12</v>
@@ -30035,7 +30035,7 @@
         <v>1.8</v>
       </c>
       <c r="E722" t="n">
-        <v>0.08800000000000001</v>
+        <v>0.08799999999999999</v>
       </c>
       <c r="F722" t="n">
         <v>12</v>
@@ -30199,7 +30199,7 @@
         <v>1.8</v>
       </c>
       <c r="E726" t="n">
-        <v>0.08800000000000001</v>
+        <v>0.08799999999999999</v>
       </c>
       <c r="F726" t="n">
         <v>12</v>
@@ -30363,7 +30363,7 @@
         <v>2.5</v>
       </c>
       <c r="E730" t="n">
-        <v>0.08199999999999999</v>
+        <v>0.08199999999999991</v>
       </c>
       <c r="F730" t="n">
         <v>26</v>
@@ -30445,7 +30445,7 @@
         <v>2.2</v>
       </c>
       <c r="E732" t="n">
-        <v>0.08800000000000001</v>
+        <v>0.08799999999999999</v>
       </c>
       <c r="F732" t="n">
         <v>21</v>
@@ -30650,7 +30650,7 @@
         <v>1.8</v>
       </c>
       <c r="E737" t="n">
-        <v>0.08199999999999999</v>
+        <v>0.08199999999999991</v>
       </c>
       <c r="F737" t="n">
         <v>27</v>
@@ -30937,7 +30937,7 @@
         <v>4</v>
       </c>
       <c r="E744" t="n">
-        <v>0.101</v>
+        <v>0.1009999999999999</v>
       </c>
       <c r="F744" t="n">
         <v>3</v>
@@ -31060,7 +31060,7 @@
         <v>4</v>
       </c>
       <c r="E747" t="n">
-        <v>0.101</v>
+        <v>0.1009999999999999</v>
       </c>
       <c r="F747" t="n">
         <v>3</v>
@@ -31101,7 +31101,7 @@
         <v>1.8</v>
       </c>
       <c r="E748" t="n">
-        <v>0.07400000000000001</v>
+        <v>0.074</v>
       </c>
       <c r="F748" t="n">
         <v>3</v>
@@ -31552,7 +31552,7 @@
         <v>2.7</v>
       </c>
       <c r="E759" t="n">
-        <v>0.08800000000000001</v>
+        <v>0.08799999999999999</v>
       </c>
       <c r="F759" t="n">
         <v>16</v>
@@ -31798,7 +31798,7 @@
         <v>2.4</v>
       </c>
       <c r="E765" t="n">
-        <v>0.07200000000000001</v>
+        <v>0.07199999999999999</v>
       </c>
       <c r="F765" t="n">
         <v>32</v>
@@ -31839,7 +31839,7 @@
         <v>1.8</v>
       </c>
       <c r="E766" t="n">
-        <v>0.07400000000000001</v>
+        <v>0.074</v>
       </c>
       <c r="F766" t="n">
         <v>40</v>
@@ -32208,7 +32208,7 @@
         <v>5.5</v>
       </c>
       <c r="E775" t="n">
-        <v>0.117</v>
+        <v>0.1169999999999999</v>
       </c>
       <c r="F775" t="n">
         <v>9</v>
@@ -32249,7 +32249,7 @@
         <v>5.5</v>
       </c>
       <c r="E776" t="n">
-        <v>0.117</v>
+        <v>0.1169999999999999</v>
       </c>
       <c r="F776" t="n">
         <v>9</v>
@@ -32331,7 +32331,7 @@
         <v>2.1</v>
       </c>
       <c r="E778" t="n">
-        <v>0.07200000000000001</v>
+        <v>0.07199999999999999</v>
       </c>
       <c r="F778" t="n">
         <v>23</v>
@@ -32741,7 +32741,7 @@
         <v>1.5</v>
       </c>
       <c r="E788" t="n">
-        <v>0.056</v>
+        <v>0.0559999999999999</v>
       </c>
       <c r="F788" t="n">
         <v>6</v>
@@ -33151,7 +33151,7 @@
         <v>2.9</v>
       </c>
       <c r="E798" t="n">
-        <v>0.07200000000000001</v>
+        <v>0.07199999999999999</v>
       </c>
       <c r="F798" t="n">
         <v>26</v>
@@ -33233,7 +33233,7 @@
         <v>1.9</v>
       </c>
       <c r="E800" t="n">
-        <v>0.058</v>
+        <v>0.0579999999999999</v>
       </c>
       <c r="F800" t="n">
         <v>5</v>
@@ -33315,7 +33315,7 @@
         <v>5.5</v>
       </c>
       <c r="E802" t="n">
-        <v>0.08900000000000001</v>
+        <v>0.089</v>
       </c>
       <c r="F802" t="n">
         <v>10</v>
@@ -34299,7 +34299,7 @@
         <v>2.5</v>
       </c>
       <c r="E826" t="n">
-        <v>0.07400000000000001</v>
+        <v>0.074</v>
       </c>
       <c r="F826" t="n">
         <v>29</v>
@@ -34463,7 +34463,7 @@
         <v>2.1</v>
       </c>
       <c r="E830" t="n">
-        <v>0.07400000000000001</v>
+        <v>0.074</v>
       </c>
       <c r="F830" t="n">
         <v>5</v>
@@ -34668,7 +34668,7 @@
         <v>2.1</v>
       </c>
       <c r="E835" t="n">
-        <v>0.041</v>
+        <v>0.0409999999999999</v>
       </c>
       <c r="F835" t="n">
         <v>17</v>
@@ -35447,7 +35447,7 @@
         <v>2.1</v>
       </c>
       <c r="E854" t="n">
-        <v>0.07400000000000001</v>
+        <v>0.074</v>
       </c>
       <c r="F854" t="n">
         <v>24</v>
@@ -35488,7 +35488,7 @@
         <v>2.1</v>
       </c>
       <c r="E855" t="n">
-        <v>0.07400000000000001</v>
+        <v>0.074</v>
       </c>
       <c r="F855" t="n">
         <v>24</v>
@@ -35570,7 +35570,7 @@
         <v>2.1</v>
       </c>
       <c r="E857" t="n">
-        <v>0.07400000000000001</v>
+        <v>0.074</v>
       </c>
       <c r="F857" t="n">
         <v>24</v>
@@ -36226,7 +36226,7 @@
         <v>2.6</v>
       </c>
       <c r="E873" t="n">
-        <v>0.07400000000000001</v>
+        <v>0.074</v>
       </c>
       <c r="F873" t="n">
         <v>48</v>
@@ -36554,7 +36554,7 @@
         <v>2.4</v>
       </c>
       <c r="E881" t="n">
-        <v>0.08199999999999999</v>
+        <v>0.08199999999999991</v>
       </c>
       <c r="F881" t="n">
         <v>10</v>
@@ -36595,7 +36595,7 @@
         <v>1.8</v>
       </c>
       <c r="E882" t="n">
-        <v>0.08199999999999999</v>
+        <v>0.08199999999999991</v>
       </c>
       <c r="F882" t="n">
         <v>15</v>
@@ -36882,7 +36882,7 @@
         <v>1.8</v>
       </c>
       <c r="E889" t="n">
-        <v>0.08199999999999999</v>
+        <v>0.08199999999999991</v>
       </c>
       <c r="F889" t="n">
         <v>43</v>
@@ -37005,7 +37005,7 @@
         <v>1.8</v>
       </c>
       <c r="E892" t="n">
-        <v>0.403</v>
+        <v>0.4029999999999999</v>
       </c>
       <c r="F892" t="n">
         <v>19</v>
@@ -38153,7 +38153,7 @@
         <v>2.4</v>
       </c>
       <c r="E920" t="n">
-        <v>0.056</v>
+        <v>0.0559999999999999</v>
       </c>
       <c r="F920" t="n">
         <v>14</v>
@@ -38317,7 +38317,7 @@
         <v>2.1</v>
       </c>
       <c r="E924" t="n">
-        <v>0.137</v>
+        <v>0.1369999999999999</v>
       </c>
       <c r="F924" t="n">
         <v>5</v>
@@ -38563,7 +38563,7 @@
         <v>2.5</v>
       </c>
       <c r="E930" t="n">
-        <v>0.08800000000000001</v>
+        <v>0.08799999999999999</v>
       </c>
       <c r="F930" t="n">
         <v>22</v>
@@ -38768,7 +38768,7 @@
         <v>1.2</v>
       </c>
       <c r="E935" t="n">
-        <v>0.041</v>
+        <v>0.0409999999999999</v>
       </c>
       <c r="F935" t="n">
         <v>16</v>
@@ -38850,7 +38850,7 @@
         <v>1.2</v>
       </c>
       <c r="E937" t="n">
-        <v>0.041</v>
+        <v>0.0409999999999999</v>
       </c>
       <c r="F937" t="n">
         <v>16</v>
@@ -38891,7 +38891,7 @@
         <v>1.8</v>
       </c>
       <c r="E938" t="n">
-        <v>0.058</v>
+        <v>0.0579999999999999</v>
       </c>
       <c r="F938" t="n">
         <v>9</v>
@@ -39793,7 +39793,7 @@
         <v>2.1</v>
       </c>
       <c r="E960" t="n">
-        <v>0.056</v>
+        <v>0.0559999999999999</v>
       </c>
       <c r="F960" t="n">
         <v>5</v>
@@ -40326,7 +40326,7 @@
         <v>2.2</v>
       </c>
       <c r="E973" t="n">
-        <v>0.08800000000000001</v>
+        <v>0.08799999999999999</v>
       </c>
       <c r="F973" t="n">
         <v>9</v>
@@ -41392,7 +41392,7 @@
         <v>2.6</v>
       </c>
       <c r="E999" t="n">
-        <v>0.08199999999999999</v>
+        <v>0.08199999999999991</v>
       </c>
       <c r="F999" t="n">
         <v>12</v>
@@ -41597,7 +41597,7 @@
         <v>1.8</v>
       </c>
       <c r="E1004" t="n">
-        <v>0.08199999999999999</v>
+        <v>0.08199999999999991</v>
       </c>
       <c r="F1004" t="n">
         <v>5</v>
@@ -42212,7 +42212,7 @@
         <v>1.9</v>
       </c>
       <c r="E1019" t="n">
-        <v>0.07200000000000001</v>
+        <v>0.07199999999999999</v>
       </c>
       <c r="F1019" t="n">
         <v>27</v>
@@ -42458,7 +42458,7 @@
         <v>1.6</v>
       </c>
       <c r="E1025" t="n">
-        <v>0.169</v>
+        <v>0.1689999999999999</v>
       </c>
       <c r="F1025" t="n">
         <v>27</v>
@@ -42581,7 +42581,7 @@
         <v>2.2</v>
       </c>
       <c r="E1028" t="n">
-        <v>0.07200000000000001</v>
+        <v>0.07199999999999999</v>
       </c>
       <c r="F1028" t="n">
         <v>31</v>
@@ -42622,7 +42622,7 @@
         <v>1.75</v>
       </c>
       <c r="E1029" t="n">
-        <v>0.058</v>
+        <v>0.0579999999999999</v>
       </c>
       <c r="F1029" t="n">
         <v>8</v>
@@ -42745,7 +42745,7 @@
         <v>2</v>
       </c>
       <c r="E1032" t="n">
-        <v>0.056</v>
+        <v>0.0559999999999999</v>
       </c>
       <c r="F1032" t="n">
         <v>15</v>
@@ -42991,7 +42991,7 @@
         <v>1.9</v>
       </c>
       <c r="E1038" t="n">
-        <v>0.07400000000000001</v>
+        <v>0.074</v>
       </c>
       <c r="F1038" t="n">
         <v>27</v>
@@ -43073,7 +43073,7 @@
         <v>1.7</v>
       </c>
       <c r="E1040" t="n">
-        <v>0.05400000000000001</v>
+        <v>0.054</v>
       </c>
       <c r="F1040" t="n">
         <v>7</v>
@@ -43114,7 +43114,7 @@
         <v>2.3</v>
       </c>
       <c r="E1041" t="n">
-        <v>0.05400000000000001</v>
+        <v>0.054</v>
       </c>
       <c r="F1041" t="n">
         <v>34</v>
@@ -43770,7 +43770,7 @@
         <v>5.7</v>
       </c>
       <c r="E1057" t="n">
-        <v>0.08199999999999999</v>
+        <v>0.08199999999999991</v>
       </c>
       <c r="F1057" t="n">
         <v>3</v>
@@ -43975,7 +43975,7 @@
         <v>2.1</v>
       </c>
       <c r="E1062" t="n">
-        <v>0.07400000000000001</v>
+        <v>0.074</v>
       </c>
       <c r="F1062" t="n">
         <v>8</v>
@@ -44221,7 +44221,7 @@
         <v>1.9</v>
       </c>
       <c r="E1068" t="n">
-        <v>0.08900000000000001</v>
+        <v>0.089</v>
       </c>
       <c r="F1068" t="n">
         <v>23</v>
@@ -44344,7 +44344,7 @@
         <v>2.3</v>
       </c>
       <c r="E1071" t="n">
-        <v>0.05400000000000001</v>
+        <v>0.054</v>
       </c>
       <c r="F1071" t="n">
         <v>7</v>
@@ -44385,7 +44385,7 @@
         <v>2.3</v>
       </c>
       <c r="E1072" t="n">
-        <v>0.05400000000000001</v>
+        <v>0.054</v>
       </c>
       <c r="F1072" t="n">
         <v>7</v>
@@ -44672,7 +44672,7 @@
         <v>2.1</v>
       </c>
       <c r="E1079" t="n">
-        <v>0.07400000000000001</v>
+        <v>0.074</v>
       </c>
       <c r="F1079" t="n">
         <v>17</v>
@@ -44836,7 +44836,7 @@
         <v>4.1</v>
       </c>
       <c r="E1083" t="n">
-        <v>0.07400000000000001</v>
+        <v>0.074</v>
       </c>
       <c r="F1083" t="n">
         <v>16</v>
@@ -44877,7 +44877,7 @@
         <v>4.1</v>
       </c>
       <c r="E1084" t="n">
-        <v>0.07400000000000001</v>
+        <v>0.074</v>
       </c>
       <c r="F1084" t="n">
         <v>16</v>
@@ -45369,7 +45369,7 @@
         <v>2</v>
       </c>
       <c r="E1096" t="n">
-        <v>0.058</v>
+        <v>0.0579999999999999</v>
       </c>
       <c r="F1096" t="n">
         <v>18</v>
@@ -45410,7 +45410,7 @@
         <v>1.9</v>
       </c>
       <c r="E1097" t="n">
-        <v>0.07400000000000001</v>
+        <v>0.074</v>
       </c>
       <c r="F1097" t="n">
         <v>32</v>
@@ -45697,7 +45697,7 @@
         <v>2</v>
       </c>
       <c r="E1104" t="n">
-        <v>0.07200000000000001</v>
+        <v>0.07199999999999999</v>
       </c>
       <c r="F1104" t="n">
         <v>17</v>
@@ -45779,7 +45779,7 @@
         <v>1.8</v>
       </c>
       <c r="E1106" t="n">
-        <v>0.07400000000000001</v>
+        <v>0.074</v>
       </c>
       <c r="F1106" t="n">
         <v>17</v>
@@ -46476,7 +46476,7 @@
         <v>1.9</v>
       </c>
       <c r="E1123" t="n">
-        <v>0.056</v>
+        <v>0.0559999999999999</v>
       </c>
       <c r="F1123" t="n">
         <v>15</v>
@@ -46927,7 +46927,7 @@
         <v>2.1</v>
       </c>
       <c r="E1134" t="n">
-        <v>0.07400000000000001</v>
+        <v>0.074</v>
       </c>
       <c r="F1134" t="n">
         <v>32</v>
@@ -47132,7 +47132,7 @@
         <v>1.7</v>
       </c>
       <c r="E1139" t="n">
-        <v>0.08900000000000001</v>
+        <v>0.089</v>
       </c>
       <c r="F1139" t="n">
         <v>16</v>

</xml_diff>